<commit_message>
Delivery details test added
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="28">
   <si>
     <t>first</t>
   </si>
@@ -556,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>